<commit_message>
template kaydederken formüller kaydediliyor
</commit_message>
<xml_diff>
--- a/WebApplication1/Forms/02_bloksaplamaları.xlsx
+++ b/WebApplication1/Forms/02_bloksaplamaları.xlsx
@@ -937,6 +937,118 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="6"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -959,9 +1071,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -972,115 +1081,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1097,88 +1097,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>381000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1025" name="Rectangle 1"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3627120" y="7117080"/>
-          <a:ext cx="632460" cy="716280"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="tr-TR" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="tr-TR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Times New Roman"/>
-              <a:cs typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>        8</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1470,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1494,21 +1412,21 @@
       <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="51" t="s">
+      <c r="D1" s="87"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="51" t="s">
+      <c r="G1" s="87"/>
+      <c r="H1" s="88"/>
+      <c r="I1" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="K1" s="53"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="88"/>
       <c r="L1" s="17" t="s">
         <v>3</v>
       </c>
@@ -1523,17 +1441,17 @@
       <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57" t="s">
+      <c r="C2" s="89"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="56"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="90"/>
+      <c r="K2" s="91"/>
       <c r="L2" s="20" t="s">
         <v>4</v>
       </c>
@@ -1555,9 +1473,9 @@
       <c r="E3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="62"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="96"/>
       <c r="I3" s="20" t="s">
         <v>9</v>
       </c>
@@ -1573,7 +1491,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="63">
+      <c r="A4" s="74">
         <v>1</v>
       </c>
       <c r="B4" s="23">
@@ -1585,9 +1503,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="73"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="85"/>
       <c r="I4" s="3"/>
       <c r="J4" s="24" t="e">
         <f xml:space="preserve"> ((I4-K4)/K4)</f>
@@ -1597,12 +1515,12 @@
       <c r="L4" s="25">
         <v>1</v>
       </c>
-      <c r="M4" s="63">
+      <c r="M4" s="74">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="64"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="26">
         <v>2</v>
       </c>
@@ -1612,9 +1530,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="70"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="72"/>
       <c r="I5" s="4"/>
       <c r="J5" s="24" t="e">
         <f xml:space="preserve"> ((I5-K5)/K5)</f>
@@ -1624,10 +1542,10 @@
       <c r="L5" s="28">
         <v>2</v>
       </c>
-      <c r="M5" s="64"/>
+      <c r="M5" s="52"/>
     </row>
     <row r="6" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="64"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="26">
         <v>3</v>
       </c>
@@ -1637,9 +1555,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="70"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="72"/>
       <c r="I6" s="4"/>
       <c r="J6" s="24" t="e">
         <f t="shared" ref="J6:J32" si="1" xml:space="preserve"> ((I6-K6)/K6)</f>
@@ -1649,10 +1567,10 @@
       <c r="L6" s="28">
         <v>3</v>
       </c>
-      <c r="M6" s="64"/>
+      <c r="M6" s="52"/>
     </row>
     <row r="7" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="65"/>
+      <c r="A7" s="53"/>
       <c r="B7" s="29">
         <v>4</v>
       </c>
@@ -1663,7 +1581,7 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="30"/>
-      <c r="G7" s="66">
+      <c r="G7" s="51">
         <v>1</v>
       </c>
       <c r="H7" s="30"/>
@@ -1676,10 +1594,10 @@
       <c r="L7" s="31">
         <v>4</v>
       </c>
-      <c r="M7" s="65"/>
+      <c r="M7" s="53"/>
     </row>
     <row r="8" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="63">
+      <c r="A8" s="74">
         <v>2</v>
       </c>
       <c r="B8" s="23">
@@ -1692,7 +1610,7 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="32"/>
-      <c r="G8" s="67"/>
+      <c r="G8" s="75"/>
       <c r="H8" s="32"/>
       <c r="I8" s="3"/>
       <c r="J8" s="24" t="e">
@@ -1703,12 +1621,12 @@
       <c r="L8" s="25">
         <v>1</v>
       </c>
-      <c r="M8" s="63">
+      <c r="M8" s="74">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="64"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="26">
         <v>2</v>
       </c>
@@ -1718,9 +1636,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="70"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="72"/>
       <c r="I9" s="4"/>
       <c r="J9" s="24" t="e">
         <f t="shared" si="1"/>
@@ -1730,10 +1648,10 @@
       <c r="L9" s="28">
         <v>2</v>
       </c>
-      <c r="M9" s="64"/>
+      <c r="M9" s="52"/>
     </row>
     <row r="10" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="64"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="26">
         <v>3</v>
       </c>
@@ -1743,9 +1661,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="70"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="72"/>
       <c r="I10" s="4"/>
       <c r="J10" s="24" t="e">
         <f t="shared" si="1"/>
@@ -1755,10 +1673,10 @@
       <c r="L10" s="28">
         <v>3</v>
       </c>
-      <c r="M10" s="64"/>
+      <c r="M10" s="52"/>
     </row>
     <row r="11" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="65"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="29">
         <v>4</v>
       </c>
@@ -1769,7 +1687,7 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="33"/>
-      <c r="G11" s="66">
+      <c r="G11" s="51">
         <v>2</v>
       </c>
       <c r="H11" s="30"/>
@@ -1782,10 +1700,10 @@
       <c r="L11" s="31">
         <v>4</v>
       </c>
-      <c r="M11" s="65"/>
+      <c r="M11" s="53"/>
     </row>
     <row r="12" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="63">
+      <c r="A12" s="74">
         <v>3</v>
       </c>
       <c r="B12" s="23">
@@ -1798,7 +1716,7 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="34"/>
-      <c r="G12" s="67"/>
+      <c r="G12" s="75"/>
       <c r="H12" s="32"/>
       <c r="I12" s="3"/>
       <c r="J12" s="24" t="e">
@@ -1809,12 +1727,12 @@
       <c r="L12" s="25">
         <v>1</v>
       </c>
-      <c r="M12" s="63">
+      <c r="M12" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="64"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="26">
         <v>2</v>
       </c>
@@ -1824,9 +1742,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="70"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="72"/>
       <c r="I13" s="4"/>
       <c r="J13" s="24" t="e">
         <f t="shared" si="1"/>
@@ -1836,10 +1754,10 @@
       <c r="L13" s="28">
         <v>2</v>
       </c>
-      <c r="M13" s="64"/>
+      <c r="M13" s="52"/>
     </row>
     <row r="14" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="64"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="26">
         <v>3</v>
       </c>
@@ -1849,9 +1767,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="70"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="72"/>
       <c r="I14" s="4"/>
       <c r="J14" s="24" t="e">
         <f t="shared" si="1"/>
@@ -1861,10 +1779,10 @@
       <c r="L14" s="28">
         <v>3</v>
       </c>
-      <c r="M14" s="64"/>
+      <c r="M14" s="52"/>
     </row>
     <row r="15" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="65"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="29">
         <v>4</v>
       </c>
@@ -1875,7 +1793,7 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="30"/>
-      <c r="G15" s="66">
+      <c r="G15" s="51">
         <v>3</v>
       </c>
       <c r="H15" s="30"/>
@@ -1888,10 +1806,10 @@
       <c r="L15" s="31">
         <v>4</v>
       </c>
-      <c r="M15" s="65"/>
+      <c r="M15" s="53"/>
     </row>
     <row r="16" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="63">
+      <c r="A16" s="74">
         <v>4</v>
       </c>
       <c r="B16" s="23">
@@ -1904,7 +1822,7 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="32"/>
-      <c r="G16" s="67"/>
+      <c r="G16" s="75"/>
       <c r="H16" s="32"/>
       <c r="I16" s="3"/>
       <c r="J16" s="24" t="e">
@@ -1915,12 +1833,12 @@
       <c r="L16" s="25">
         <v>1</v>
       </c>
-      <c r="M16" s="63">
+      <c r="M16" s="74">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="64"/>
+      <c r="A17" s="52"/>
       <c r="B17" s="26">
         <v>2</v>
       </c>
@@ -1930,9 +1848,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="70"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="72"/>
       <c r="I17" s="4"/>
       <c r="J17" s="24" t="e">
         <f t="shared" si="1"/>
@@ -1942,10 +1860,10 @@
       <c r="L17" s="28">
         <v>2</v>
       </c>
-      <c r="M17" s="64"/>
+      <c r="M17" s="52"/>
     </row>
     <row r="18" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="64"/>
+      <c r="A18" s="52"/>
       <c r="B18" s="26">
         <v>3</v>
       </c>
@@ -1955,9 +1873,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="70"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="72"/>
       <c r="I18" s="4"/>
       <c r="J18" s="24" t="e">
         <f t="shared" si="1"/>
@@ -1967,10 +1885,10 @@
       <c r="L18" s="28">
         <v>3</v>
       </c>
-      <c r="M18" s="64"/>
+      <c r="M18" s="52"/>
     </row>
     <row r="19" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="65"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="29">
         <v>4</v>
       </c>
@@ -1981,7 +1899,7 @@
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="30"/>
-      <c r="G19" s="66">
+      <c r="G19" s="51">
         <v>4</v>
       </c>
       <c r="H19" s="30"/>
@@ -1994,10 +1912,10 @@
       <c r="L19" s="31">
         <v>4</v>
       </c>
-      <c r="M19" s="65"/>
+      <c r="M19" s="53"/>
     </row>
     <row r="20" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="63">
+      <c r="A20" s="74">
         <v>5</v>
       </c>
       <c r="B20" s="23">
@@ -2010,7 +1928,7 @@
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="32"/>
-      <c r="G20" s="67"/>
+      <c r="G20" s="75"/>
       <c r="H20" s="32"/>
       <c r="I20" s="3"/>
       <c r="J20" s="24" t="e">
@@ -2021,12 +1939,12 @@
       <c r="L20" s="25">
         <v>1</v>
       </c>
-      <c r="M20" s="63">
+      <c r="M20" s="74">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="64"/>
+      <c r="A21" s="52"/>
       <c r="B21" s="26">
         <v>2</v>
       </c>
@@ -2036,9 +1954,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="70"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="72"/>
       <c r="I21" s="4"/>
       <c r="J21" s="24" t="e">
         <f xml:space="preserve"> ((I21-K21)/K21)</f>
@@ -2048,10 +1966,10 @@
       <c r="L21" s="28">
         <v>2</v>
       </c>
-      <c r="M21" s="64"/>
+      <c r="M21" s="52"/>
     </row>
     <row r="22" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="64"/>
+      <c r="A22" s="52"/>
       <c r="B22" s="26">
         <v>3</v>
       </c>
@@ -2061,9 +1979,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="70"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="72"/>
       <c r="I22" s="4"/>
       <c r="J22" s="24" t="e">
         <f t="shared" si="1"/>
@@ -2073,10 +1991,10 @@
       <c r="L22" s="28">
         <v>3</v>
       </c>
-      <c r="M22" s="64"/>
+      <c r="M22" s="52"/>
     </row>
     <row r="23" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="65"/>
+      <c r="A23" s="53"/>
       <c r="B23" s="29">
         <v>4</v>
       </c>
@@ -2087,7 +2005,7 @@
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="30"/>
-      <c r="G23" s="66">
+      <c r="G23" s="51">
         <v>5</v>
       </c>
       <c r="H23" s="30"/>
@@ -2100,10 +2018,10 @@
       <c r="L23" s="31">
         <v>4</v>
       </c>
-      <c r="M23" s="65"/>
+      <c r="M23" s="53"/>
     </row>
     <row r="24" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="63">
+      <c r="A24" s="74">
         <v>6</v>
       </c>
       <c r="B24" s="23">
@@ -2116,7 +2034,7 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="32"/>
-      <c r="G24" s="67"/>
+      <c r="G24" s="75"/>
       <c r="H24" s="32"/>
       <c r="I24" s="3"/>
       <c r="J24" s="24" t="e">
@@ -2127,12 +2045,12 @@
       <c r="L24" s="25">
         <v>1</v>
       </c>
-      <c r="M24" s="63">
+      <c r="M24" s="74">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="64"/>
+      <c r="A25" s="52"/>
       <c r="B25" s="26">
         <v>2</v>
       </c>
@@ -2142,9 +2060,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="70"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="72"/>
       <c r="I25" s="4"/>
       <c r="J25" s="24" t="e">
         <f t="shared" si="1"/>
@@ -2154,10 +2072,10 @@
       <c r="L25" s="28">
         <v>2</v>
       </c>
-      <c r="M25" s="64"/>
+      <c r="M25" s="52"/>
     </row>
     <row r="26" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="64"/>
+      <c r="A26" s="52"/>
       <c r="B26" s="26">
         <v>3</v>
       </c>
@@ -2167,9 +2085,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="70"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="72"/>
       <c r="I26" s="4"/>
       <c r="J26" s="24" t="e">
         <f t="shared" si="1"/>
@@ -2179,10 +2097,10 @@
       <c r="L26" s="28">
         <v>3</v>
       </c>
-      <c r="M26" s="64"/>
+      <c r="M26" s="52"/>
     </row>
     <row r="27" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="65"/>
+      <c r="A27" s="53"/>
       <c r="B27" s="29">
         <v>4</v>
       </c>
@@ -2193,7 +2111,7 @@
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="30"/>
-      <c r="G27" s="66">
+      <c r="G27" s="51">
         <v>6</v>
       </c>
       <c r="H27" s="30"/>
@@ -2206,10 +2124,10 @@
       <c r="L27" s="31">
         <v>4</v>
       </c>
-      <c r="M27" s="65"/>
+      <c r="M27" s="53"/>
     </row>
     <row r="28" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="63">
+      <c r="A28" s="74">
         <v>7</v>
       </c>
       <c r="B28" s="23">
@@ -2222,7 +2140,7 @@
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="32"/>
-      <c r="G28" s="67"/>
+      <c r="G28" s="75"/>
       <c r="H28" s="32"/>
       <c r="I28" s="3"/>
       <c r="J28" s="24" t="e">
@@ -2233,12 +2151,12 @@
       <c r="L28" s="25">
         <v>1</v>
       </c>
-      <c r="M28" s="63">
+      <c r="M28" s="74">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="64"/>
+      <c r="A29" s="52"/>
       <c r="B29" s="26">
         <v>2</v>
       </c>
@@ -2248,9 +2166,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="70"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="72"/>
       <c r="I29" s="4"/>
       <c r="J29" s="24" t="e">
         <f t="shared" si="1"/>
@@ -2260,10 +2178,10 @@
       <c r="L29" s="28">
         <v>2</v>
       </c>
-      <c r="M29" s="64"/>
+      <c r="M29" s="52"/>
     </row>
     <row r="30" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="64"/>
+      <c r="A30" s="52"/>
       <c r="B30" s="26">
         <v>3</v>
       </c>
@@ -2273,9 +2191,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="70"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="72"/>
       <c r="I30" s="4"/>
       <c r="J30" s="24" t="e">
         <f xml:space="preserve"> ((I30-K30)/K30)</f>
@@ -2285,10 +2203,10 @@
       <c r="L30" s="28">
         <v>3</v>
       </c>
-      <c r="M30" s="64"/>
+      <c r="M30" s="52"/>
     </row>
     <row r="31" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="65"/>
+      <c r="A31" s="53"/>
       <c r="B31" s="29">
         <v>4</v>
       </c>
@@ -2299,7 +2217,7 @@
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="33"/>
-      <c r="G31" s="66">
+      <c r="G31" s="51">
         <v>7</v>
       </c>
       <c r="H31" s="30"/>
@@ -2312,10 +2230,10 @@
       <c r="L31" s="31">
         <v>4</v>
       </c>
-      <c r="M31" s="65"/>
+      <c r="M31" s="53"/>
     </row>
     <row r="32" spans="1:13" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="63">
+      <c r="A32" s="74">
         <v>8</v>
       </c>
       <c r="B32" s="23">
@@ -2328,7 +2246,7 @@
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="34"/>
-      <c r="G32" s="67"/>
+      <c r="G32" s="75"/>
       <c r="H32" s="32"/>
       <c r="I32" s="7"/>
       <c r="J32" s="35" t="e">
@@ -2339,112 +2257,112 @@
       <c r="L32" s="36">
         <v>1</v>
       </c>
-      <c r="M32" s="63">
+      <c r="M32" s="74">
         <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="64"/>
-      <c r="B33" s="75">
+      <c r="A33" s="52"/>
+      <c r="B33" s="77">
         <v>2</v>
       </c>
-      <c r="C33" s="78"/>
-      <c r="D33" s="82" t="e">
+      <c r="C33" s="80"/>
+      <c r="D33" s="55" t="e">
         <f>(E33-C33)/E33</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E33" s="85"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="92" t="e">
+      <c r="E33" s="58"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="68" t="e">
         <f>(K33-I33)/K33</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K33" s="91"/>
-      <c r="L33" s="96">
+      <c r="K33" s="67"/>
+      <c r="L33" s="73">
         <v>2</v>
       </c>
-      <c r="M33" s="59"/>
+      <c r="M33" s="76"/>
     </row>
     <row r="34" spans="1:13" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="64"/>
-      <c r="B34" s="76"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="86"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="91"/>
-      <c r="J34" s="92"/>
-      <c r="K34" s="91"/>
-      <c r="L34" s="96"/>
-      <c r="M34" s="59"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="68"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="76"/>
     </row>
     <row r="35" spans="1:13" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="64"/>
-      <c r="B35" s="76"/>
-      <c r="C35" s="79"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="74"/>
-      <c r="I35" s="91"/>
-      <c r="J35" s="92"/>
-      <c r="K35" s="91"/>
-      <c r="L35" s="96"/>
-      <c r="M35" s="59"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="63"/>
+      <c r="I35" s="67"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="73"/>
+      <c r="M35" s="76"/>
     </row>
     <row r="36" spans="1:13" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="64"/>
-      <c r="B36" s="76"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="91"/>
-      <c r="J36" s="92"/>
-      <c r="K36" s="91"/>
-      <c r="L36" s="96"/>
-      <c r="M36" s="59"/>
+      <c r="A36" s="52"/>
+      <c r="B36" s="78"/>
+      <c r="C36" s="81"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="68"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="73"/>
+      <c r="M36" s="76"/>
     </row>
     <row r="37" spans="1:13" ht="15.6" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="64"/>
-      <c r="B37" s="76"/>
-      <c r="C37" s="79"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="74"/>
-      <c r="I37" s="91"/>
-      <c r="J37" s="92"/>
-      <c r="K37" s="91"/>
-      <c r="L37" s="96"/>
-      <c r="M37" s="59"/>
+      <c r="A37" s="52"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="68"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="73"/>
+      <c r="M37" s="76"/>
     </row>
     <row r="38" spans="1:13" ht="15.6" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="64"/>
-      <c r="B38" s="77"/>
-      <c r="C38" s="80"/>
-      <c r="D38" s="84"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="91"/>
-      <c r="J38" s="92"/>
-      <c r="K38" s="91"/>
-      <c r="L38" s="96"/>
-      <c r="M38" s="59"/>
+      <c r="A38" s="52"/>
+      <c r="B38" s="79"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="67"/>
+      <c r="J38" s="68"/>
+      <c r="K38" s="67"/>
+      <c r="L38" s="73"/>
+      <c r="M38" s="76"/>
     </row>
     <row r="39" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="64"/>
+      <c r="A39" s="52"/>
       <c r="B39" s="26">
         <v>3</v>
       </c>
@@ -2454,9 +2372,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E39" s="4"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="69"/>
-      <c r="H39" s="74"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="63"/>
       <c r="I39" s="15"/>
       <c r="J39" s="37" t="e">
         <f>(K39-I39)/K39</f>
@@ -2466,10 +2384,10 @@
       <c r="L39" s="38">
         <v>3</v>
       </c>
-      <c r="M39" s="59"/>
+      <c r="M39" s="76"/>
     </row>
     <row r="40" spans="1:13" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="67"/>
+      <c r="A40" s="75"/>
       <c r="B40" s="26">
         <v>4</v>
       </c>
@@ -2479,9 +2397,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E40" s="4"/>
-      <c r="F40" s="88"/>
-      <c r="G40" s="89"/>
-      <c r="H40" s="90"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="66"/>
       <c r="I40" s="4"/>
       <c r="J40" s="37" t="e">
         <f t="shared" ref="J40:J44" si="2">(K40-I40)/K40</f>
@@ -2491,10 +2409,10 @@
       <c r="L40" s="28">
         <v>4</v>
       </c>
-      <c r="M40" s="67"/>
+      <c r="M40" s="75"/>
     </row>
     <row r="41" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="66">
+      <c r="A41" s="51">
         <v>9</v>
       </c>
       <c r="B41" s="26">
@@ -2506,9 +2424,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E41" s="4"/>
-      <c r="F41" s="93"/>
-      <c r="G41" s="94"/>
-      <c r="H41" s="95"/>
+      <c r="F41" s="69"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="71"/>
       <c r="I41" s="4"/>
       <c r="J41" s="37" t="e">
         <f t="shared" si="2"/>
@@ -2518,12 +2436,12 @@
       <c r="L41" s="28">
         <v>1</v>
       </c>
-      <c r="M41" s="66">
+      <c r="M41" s="51">
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="64"/>
+      <c r="A42" s="52"/>
       <c r="B42" s="26">
         <v>2</v>
       </c>
@@ -2533,9 +2451,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E42" s="4"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="70"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="72"/>
       <c r="I42" s="4"/>
       <c r="J42" s="37" t="e">
         <f t="shared" si="2"/>
@@ -2545,10 +2463,10 @@
       <c r="L42" s="28">
         <v>2</v>
       </c>
-      <c r="M42" s="64"/>
+      <c r="M42" s="52"/>
     </row>
     <row r="43" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="64"/>
+      <c r="A43" s="52"/>
       <c r="B43" s="26">
         <v>3</v>
       </c>
@@ -2558,9 +2476,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="70"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="72"/>
       <c r="I43" s="4"/>
       <c r="J43" s="37" t="e">
         <f t="shared" si="2"/>
@@ -2570,10 +2488,10 @@
       <c r="L43" s="28">
         <v>3</v>
       </c>
-      <c r="M43" s="64"/>
+      <c r="M43" s="52"/>
     </row>
     <row r="44" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="65"/>
+      <c r="A44" s="53"/>
       <c r="B44" s="39">
         <v>4</v>
       </c>
@@ -2583,9 +2501,9 @@
         <v>#DIV/0!</v>
       </c>
       <c r="E44" s="6"/>
-      <c r="F44" s="88"/>
-      <c r="G44" s="89"/>
-      <c r="H44" s="90"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="66"/>
       <c r="I44" s="6"/>
       <c r="J44" s="37" t="e">
         <f t="shared" si="2"/>
@@ -2595,7 +2513,7 @@
       <c r="L44" s="40">
         <v>4</v>
       </c>
-      <c r="M44" s="65"/>
+      <c r="M44" s="53"/>
     </row>
     <row r="45" spans="1:13" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A45" s="41" t="s">
@@ -2652,19 +2570,19 @@
       <c r="A51" s="50"/>
     </row>
     <row r="52" spans="1:10" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="81" t="s">
+      <c r="A52" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B52" s="81"/>
-      <c r="C52" s="81"/>
-      <c r="D52" s="81"/>
-      <c r="F52" s="81" t="s">
+      <c r="B52" s="54"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
+      <c r="F52" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="G52" s="81"/>
-      <c r="H52" s="81"/>
-      <c r="I52" s="81"/>
-      <c r="J52" s="81"/>
+      <c r="G52" s="54"/>
+      <c r="H52" s="54"/>
+      <c r="I52" s="54"/>
+      <c r="J52" s="54"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="29" t="s">
@@ -2680,18 +2598,27 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="49">
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="F52:J52"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="M41:M44"/>
-    <mergeCell ref="D33:D38"/>
-    <mergeCell ref="E33:E38"/>
-    <mergeCell ref="F33:H40"/>
-    <mergeCell ref="I33:I38"/>
-    <mergeCell ref="J33:J38"/>
-    <mergeCell ref="K33:K38"/>
-    <mergeCell ref="F41:H44"/>
-    <mergeCell ref="L33:L38"/>
+    <mergeCell ref="C1:E2"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I1:K2"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="M8:M11"/>
+    <mergeCell ref="F9:H10"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="F13:H14"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="F4:H6"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="M16:M19"/>
+    <mergeCell ref="F17:H18"/>
+    <mergeCell ref="G19:G20"/>
     <mergeCell ref="A20:A23"/>
     <mergeCell ref="M20:M23"/>
     <mergeCell ref="F21:H22"/>
@@ -2708,30 +2635,20 @@
     <mergeCell ref="M32:M40"/>
     <mergeCell ref="B33:B38"/>
     <mergeCell ref="C33:C38"/>
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="M8:M11"/>
-    <mergeCell ref="F9:H10"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="F13:H14"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="F4:H6"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="M16:M19"/>
-    <mergeCell ref="F17:H18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="C1:E2"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I1:K2"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="F52:J52"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="M41:M44"/>
+    <mergeCell ref="D33:D38"/>
+    <mergeCell ref="E33:E38"/>
+    <mergeCell ref="F33:H40"/>
+    <mergeCell ref="I33:I38"/>
+    <mergeCell ref="J33:J38"/>
+    <mergeCell ref="K33:K38"/>
+    <mergeCell ref="F41:H44"/>
+    <mergeCell ref="L33:L38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>